<commit_message>
Web đặt vé xem phim và quản lý
</commit_message>
<xml_diff>
--- a/docs/intro.xlsx
+++ b/docs/intro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATN_NGUYEN_CHI_THANH\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756DF2F2-BA0B-4BA4-A0E0-47F808E31595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E8B00F-97E3-40C9-AE2D-C80BF5257D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,14 +45,13 @@
     <t>Nguyễn Chí Thành</t>
   </si>
   <si>
-    <t>Hệ thống kiểm thử tự động được xây dựng nhằm giảm thời gian kiểm thử thủ công, nâng cao độ chính xác và đảm bảo chất lượng phần mềm. Đề tài áp dụng các công cụ và công nghệ phổ biến để tự động hóa quá trình kiểm thử web, từ đó giúp nhóm phát triển nhanh chóng phát hiện và khắc phục lỗi</t>
-  </si>
-  <si>
-    <t>Tự động đăng nhập vào hệ thống.
-Kiểm thử các chức năng CRUD (Create, Read, Update, Delete).</t>
-  </si>
-  <si>
-    <t>Xây dựng hệ thống kiểm thử tự động với Webdriver và Selenium</t>
+    <t xml:space="preserve">web đặt vé xem phim và trang admin quản lý </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Người dùng có thể vào tìm kiếm và đặt vé các phim muốn xem , thanh toán trực tuyến bằng vnpay   . Admin có thể quản lý phim chiếu , doanh thu</t>
+  </si>
+  <si>
+    <t>Người dùng : Chọn phim , chọn chỗ ngồi , đặt vé , thanh toán onl , xem lại lịch sử , khi thanh toán xong hiện ra hóa đơn                                                                                Admin : xếp phòng chiếu , lịch chiếu , giờ chiếu cho các phim , thống kê doanh thu theo tháng , quý . Xem thống kê tăng giảm doanh thu giữa 2 tháng liền kề hoặc 2 quý liền kề</t>
   </si>
 </sst>
 </file>
@@ -105,11 +104,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -394,55 +393,55 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="46.1796875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="18.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>191667</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="137.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>